<commit_message>
readme and contribution added
</commit_message>
<xml_diff>
--- a/101_Contribution.xlsx
+++ b/101_Contribution.xlsx
@@ -1,21 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23426"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\abc\PycharmProjects\dsadassignment\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\abc\PycharmProjects\dsadassignment\101_A1_PS17_CorpNetwork\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{902E2751-A721-435D-ADE9-62646F646147}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{3D50FCE3-58D2-41AE-AF1F-B5E1A6247D8C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{3EE97A8F-DDA8-4666-9E91-3291A22DD09A}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{E6923EAB-E42D-4220-A84A-E0919B599F0E}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="181029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -24,9 +24,50 @@
 </workbook>
 </file>
 
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="12">
+  <si>
+    <t>Group No</t>
+  </si>
+  <si>
+    <t>Name</t>
+  </si>
+  <si>
+    <t>Student Email id</t>
+  </si>
+  <si>
+    <t>% Contribution</t>
+  </si>
+  <si>
+    <t>2020ab02301@wilp.bits-pilani.ac.in</t>
+  </si>
+  <si>
+    <t>2020ab02305@wilp.bits-pilani.ac.in</t>
+  </si>
+  <si>
+    <t>Replace the above details with the details of your group.</t>
+  </si>
+  <si>
+    <t>Full (100%)</t>
+  </si>
+  <si>
+    <t>Vivek Biradar</t>
+  </si>
+  <si>
+    <t>Patil Atul Vilas</t>
+  </si>
+  <si>
+    <t>Vikrant Kumar Singh</t>
+  </si>
+  <si>
+    <t>2020fc04272@wilp.bits-pilani.ac.in</t>
+  </si>
+</sst>
+</file>
+
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -34,16 +75,34 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF92D050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -51,12 +110,36 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyProtection="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -370,13 +453,90 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4C54986F-8E70-41D1-B96D-0D042FAB0F92}">
-  <dimension ref="A1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{51BD6D89-990D-4C1E-80F5-1FED7E2030D9}">
+  <dimension ref="A1:D6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <sheetData/>
+  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="11.88671875" style="1" customWidth="1"/>
+    <col min="2" max="2" width="20.77734375" style="1" customWidth="1"/>
+    <col min="3" max="3" width="24.21875" style="1" customWidth="1"/>
+    <col min="4" max="4" width="13.33203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="16384" width="8.77734375" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A1" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="4" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A2" s="2">
+        <v>101</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A3" s="2">
+        <v>101</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A4" s="2">
+        <v>101</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A6" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+  </sheetData>
+  <sheetProtection algorithmName="SHA-512" hashValue="VgCHN9EB+CbRn73OGMmTPhJGX10wSgZUvomvIGmTUFxba8+cUgznmp5ETWE3ESuDw0pcdwoNDu87Rc5V4mdE/g==" saltValue="PGxb/+GQOO85O7Cj9FSQig==" spinCount="100000" sheet="1" objects="1" scenarios="1"/>
+  <dataValidations count="1">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D2:D4" xr:uid="{585D04A2-0E36-441C-B327-3FD50FD01BD8}">
+      <formula1>"Full (100%), Partial (50%), None (0%)"</formula1>
+    </dataValidation>
+  </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>